<commit_message>
Corrected key and code to rename columns
</commit_message>
<xml_diff>
--- a/outputs/column_names.xlsx
+++ b/outputs/column_names.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6500"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="225">
   <si>
     <t>Austria</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Ref.no</t>
   </si>
   <si>
-    <t>grid_ref_number</t>
-  </si>
-  <si>
     <t>waarneming_uri</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>species_scientific_name</t>
-  </si>
-  <si>
     <t>soort_nl</t>
   </si>
   <si>
@@ -183,547 +177,550 @@
     <t>entry_date</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>datum_schaal</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>Larve</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>heure debut</t>
+  </si>
+  <si>
+    <t>maille10km</t>
+  </si>
+  <si>
+    <t>Kartierer_Name</t>
+  </si>
+  <si>
+    <t>utm1long</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>duree</t>
+  </si>
+  <si>
+    <t>commune</t>
+  </si>
+  <si>
+    <t>Jahr_bis</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>yyyy</t>
+  </si>
+  <si>
+    <t>loc_schaal</t>
+  </si>
+  <si>
+    <t>insee_commune</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>Monat_bis</t>
+  </si>
+  <si>
+    <t>lifestage</t>
+  </si>
+  <si>
+    <t>LONG</t>
+  </si>
+  <si>
+    <t>aantal</t>
+  </si>
+  <si>
+    <t>code_postal</t>
+  </si>
+  <si>
+    <t>Tag_bis</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>stadium</t>
+  </si>
+  <si>
+    <t>nom_commune</t>
+  </si>
+  <si>
+    <t>autochtonie</t>
+  </si>
+  <si>
+    <t>X_Koordinate_komma</t>
+  </si>
+  <si>
+    <t>Record.type</t>
+  </si>
+  <si>
+    <t>waarnemer_uri</t>
+  </si>
+  <si>
+    <t>effectif</t>
+  </si>
+  <si>
+    <t>jdd</t>
+  </si>
+  <si>
+    <t>Y_Koordinate_komma</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>effectif_max</t>
+  </si>
+  <si>
+    <t>Ortsbezeichnung</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>id_observateur</t>
+  </si>
+  <si>
+    <t>observateur</t>
+  </si>
+  <si>
+    <t>Staat</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>Recorder</t>
+  </si>
+  <si>
+    <t>statut_validation</t>
+  </si>
+  <si>
+    <t>utm1</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>protocole</t>
+  </si>
+  <si>
+    <t>validateur_atlas</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>id_site</t>
+  </si>
+  <si>
+    <t>date_validation_atlas</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>Location.name</t>
+  </si>
+  <si>
+    <t>nom_site</t>
+  </si>
+  <si>
+    <t>submunicipality</t>
+  </si>
+  <si>
+    <t>Recorders</t>
+  </si>
+  <si>
+    <t>habitat aqua 1</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>eau aqua 1</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>vegetation aqua 1</t>
+  </si>
+  <si>
+    <t>certain</t>
+  </si>
+  <si>
+    <t>rives aqua 1</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>habitat aqua 2</t>
+  </si>
+  <si>
+    <t>embargo_date</t>
+  </si>
+  <si>
+    <t>eau aqua 2</t>
+  </si>
+  <si>
+    <t>permission_observer</t>
+  </si>
+  <si>
+    <t>vegetation aqua 2</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>rives aqua 2</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>habitat aqua 3</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>eau aqua 3</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
+  </si>
+  <si>
+    <t>vegetation aqua 3</t>
+  </si>
+  <si>
+    <t>id_species</t>
+  </si>
+  <si>
+    <t>rives aqua 3</t>
+  </si>
+  <si>
+    <t>id_species_type</t>
+  </si>
+  <si>
+    <t>habitat terre 1</t>
+  </si>
+  <si>
+    <t>id_checklist</t>
+  </si>
+  <si>
+    <t>habitat terre 2</t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>habitat terre 3</t>
+  </si>
+  <si>
+    <t>type_transect</t>
+  </si>
+  <si>
+    <t>activites humaines</t>
+  </si>
+  <si>
+    <t>vent</t>
+  </si>
+  <si>
+    <t>lon centroid site</t>
+  </si>
+  <si>
+    <t>lat centroid site</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>scientificName</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>taxonRank</t>
+  </si>
+  <si>
+    <t>Use controlled vocabulary (cf DwC page); usually will be species</t>
+  </si>
+  <si>
+    <t>vernacularName</t>
+  </si>
+  <si>
+    <t>recordedBy</t>
+  </si>
+  <si>
+    <t>scientificNameID</t>
+  </si>
+  <si>
+    <t>eventDate</t>
+  </si>
+  <si>
+    <t>lifeStage</t>
+  </si>
+  <si>
+    <t>lifeStage_count_a</t>
+  </si>
+  <si>
+    <t>lifeStage_count_e</t>
+  </si>
+  <si>
+    <t>lifeStage_count_l</t>
+  </si>
+  <si>
+    <t>decimalLatitude</t>
+  </si>
+  <si>
+    <t>decimalLongitude</t>
+  </si>
+  <si>
+    <t>verbatimCoordinates</t>
+  </si>
+  <si>
+    <t>verbatimLatitude</t>
+  </si>
+  <si>
+    <t>verbatimLongitude</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>eventID</t>
+  </si>
+  <si>
+    <t>individualCount</t>
+  </si>
+  <si>
+    <t>verbatimElevation</t>
+  </si>
+  <si>
+    <t>identificationVerificationStatus</t>
+  </si>
+  <si>
+    <t>entryDate</t>
+  </si>
+  <si>
+    <t>not DwC</t>
+  </si>
+  <si>
+    <t>behavior</t>
+  </si>
+  <si>
+    <t>Belgium2: is not the only info present (also vitality and comments)</t>
+  </si>
+  <si>
+    <t>samplingMethod</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>accessRights</t>
+  </si>
+  <si>
+    <t>embargoDate</t>
+  </si>
+  <si>
+    <t>occurrenceRemarks</t>
+  </si>
+  <si>
+    <t>coordinateUncertaintyInMeters</t>
+  </si>
+  <si>
+    <t>deliveryDate</t>
+  </si>
+  <si>
+    <t>samplingProtocol</t>
+  </si>
+  <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>gridRef</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>nameAccordingTo</t>
+  </si>
+  <si>
+    <t>namePublishedInYear</t>
+  </si>
+  <si>
+    <t>Jahr</t>
+  </si>
+  <si>
+    <t>associatedMedia</t>
+  </si>
+  <si>
+    <t>recordedByID</t>
+  </si>
+  <si>
+    <t>eventDateUncertainty</t>
+  </si>
+  <si>
+    <t>eventTime</t>
+  </si>
+  <si>
+    <t>samplingEffort</t>
+  </si>
+  <si>
+    <t>municipalityID</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>degreeOfEstablishment</t>
+  </si>
+  <si>
+    <t>datasetName</t>
+  </si>
+  <si>
+    <t>species_id</t>
+  </si>
+  <si>
+    <t>srt_scientific</t>
+  </si>
+  <si>
+    <t>cbs_species_id</t>
+  </si>
+  <si>
+    <t>Beleidsstatus</t>
+  </si>
+  <si>
+    <t>for STELI and OPIE taxon is longer, for Netherlands scientific name comes from other file (merged)</t>
+  </si>
+  <si>
+    <t>occurrenceID</t>
+  </si>
+  <si>
+    <t>Location_name</t>
+  </si>
+  <si>
+    <t>habitat_aqua_1</t>
+  </si>
+  <si>
+    <t>vegetation_aqua_1</t>
+  </si>
+  <si>
+    <t>rives_aqua_1</t>
+  </si>
+  <si>
+    <t>habitat_aqua_2</t>
+  </si>
+  <si>
+    <t>eau_aqua_2</t>
+  </si>
+  <si>
+    <t>vegetation_aqua_2</t>
+  </si>
+  <si>
+    <t>rives_aqua_2</t>
+  </si>
+  <si>
+    <t>habitat_aqua_3</t>
+  </si>
+  <si>
+    <t>eau_aqua_3</t>
+  </si>
+  <si>
+    <t>vegetation_aqua_3</t>
+  </si>
+  <si>
+    <t>rives_aqua_3</t>
+  </si>
+  <si>
+    <t>habitat_terre_1</t>
+  </si>
+  <si>
+    <t>habitat_terre_2</t>
+  </si>
+  <si>
+    <t>habitat_terre_3</t>
+  </si>
+  <si>
+    <t>activites_humaines</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>E dec deg</t>
+  </si>
+  <si>
+    <t>N dec deg</t>
+  </si>
+  <si>
+    <t>E deg min sec</t>
+  </si>
+  <si>
+    <t>N deg min sec</t>
+  </si>
+  <si>
+    <t>Location name</t>
+  </si>
+  <si>
+    <t>Altitude m asl</t>
+  </si>
+  <si>
+    <t>Ref no</t>
+  </si>
+  <si>
+    <t>Adult total</t>
+  </si>
+  <si>
     <t>Exuviae</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>datum_schaal</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>Larve</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>stage</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>heure debut</t>
-  </si>
-  <si>
-    <t>maille10km</t>
-  </si>
-  <si>
-    <t>Kartierer_Name</t>
-  </si>
-  <si>
-    <t>utm1long</t>
-  </si>
-  <si>
-    <t>activity</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>duree</t>
-  </si>
-  <si>
-    <t>commune</t>
-  </si>
-  <si>
-    <t>Jahr_bis</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>yyyy</t>
-  </si>
-  <si>
-    <t>larvae</t>
-  </si>
-  <si>
-    <t>loc_schaal</t>
-  </si>
-  <si>
-    <t>insee_commune</t>
-  </si>
-  <si>
-    <t>altitude</t>
-  </si>
-  <si>
-    <t>Monat_bis</t>
-  </si>
-  <si>
-    <t>lifestage</t>
-  </si>
-  <si>
-    <t>LONG</t>
-  </si>
-  <si>
-    <t>exuviae</t>
-  </si>
-  <si>
-    <t>aantal</t>
-  </si>
-  <si>
-    <t>code_postal</t>
-  </si>
-  <si>
-    <t>Tag_bis</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>LAT</t>
-  </si>
-  <si>
-    <t>x_coord</t>
-  </si>
-  <si>
-    <t>stadium</t>
-  </si>
-  <si>
-    <t>nom_commune</t>
-  </si>
-  <si>
-    <t>autochtonie</t>
-  </si>
-  <si>
-    <t>X_Koordinate_komma</t>
-  </si>
-  <si>
-    <t>Record.type</t>
-  </si>
-  <si>
-    <t>y_coord</t>
-  </si>
-  <si>
-    <t>waarnemer_uri</t>
-  </si>
-  <si>
-    <t>effectif</t>
-  </si>
-  <si>
-    <t>jdd</t>
-  </si>
-  <si>
-    <t>Y_Koordinate_komma</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>longitude_ms</t>
-  </si>
-  <si>
-    <t>effectif_max</t>
-  </si>
-  <si>
-    <t>Ortsbezeichnung</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>latitude_ms</t>
-  </si>
-  <si>
-    <t>id_observateur</t>
-  </si>
-  <si>
-    <t>observateur</t>
-  </si>
-  <si>
-    <t>Staat</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>Recorder</t>
-  </si>
-  <si>
-    <t>location_name</t>
-  </si>
-  <si>
-    <t>statut_validation</t>
-  </si>
-  <si>
-    <t>utm1</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>altitutde_m</t>
-  </si>
-  <si>
-    <t>protocole</t>
-  </si>
-  <si>
-    <t>validateur_atlas</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>id_site</t>
-  </si>
-  <si>
-    <t>date_validation_atlas</t>
-  </si>
-  <si>
-    <t>municipality</t>
-  </si>
-  <si>
-    <t>Location.name</t>
-  </si>
-  <si>
-    <t>nom_site</t>
-  </si>
-  <si>
-    <t>submunicipality</t>
-  </si>
-  <si>
-    <t>Recorders</t>
-  </si>
-  <si>
-    <t>habitat aqua 1</t>
-  </si>
-  <si>
-    <t>province</t>
-  </si>
-  <si>
-    <t>eau aqua 1</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>vegetation aqua 1</t>
-  </si>
-  <si>
-    <t>certain</t>
-  </si>
-  <si>
-    <t>rives aqua 1</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>habitat aqua 2</t>
-  </si>
-  <si>
-    <t>embargo_date</t>
-  </si>
-  <si>
-    <t>eau aqua 2</t>
-  </si>
-  <si>
-    <t>permission_observer</t>
-  </si>
-  <si>
-    <t>vegetation aqua 2</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>rives aqua 2</t>
-  </si>
-  <si>
-    <t>precision</t>
-  </si>
-  <si>
-    <t>habitat aqua 3</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>eau aqua 3</t>
-  </si>
-  <si>
-    <t>delivery_date</t>
-  </si>
-  <si>
-    <t>vegetation aqua 3</t>
-  </si>
-  <si>
-    <t>id_species</t>
-  </si>
-  <si>
-    <t>rives aqua 3</t>
-  </si>
-  <si>
-    <t>id_species_type</t>
-  </si>
-  <si>
-    <t>habitat terre 1</t>
-  </si>
-  <si>
-    <t>id_checklist</t>
-  </si>
-  <si>
-    <t>habitat terre 2</t>
-  </si>
-  <si>
-    <t>transect</t>
-  </si>
-  <si>
-    <t>habitat terre 3</t>
-  </si>
-  <si>
-    <t>type_transect</t>
-  </si>
-  <si>
-    <t>activites humaines</t>
-  </si>
-  <si>
-    <t>vent</t>
-  </si>
-  <si>
-    <t>lon centroid site</t>
-  </si>
-  <si>
-    <t>lat centroid site</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>scientificName</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>taxonRank</t>
-  </si>
-  <si>
-    <t>Use controlled vocabulary (cf DwC page); usually will be species</t>
-  </si>
-  <si>
-    <t>vernacularName</t>
-  </si>
-  <si>
-    <t>recordedBy</t>
-  </si>
-  <si>
-    <t>scientificNameID</t>
-  </si>
-  <si>
-    <t>eventDate</t>
-  </si>
-  <si>
-    <t>lifeStage</t>
-  </si>
-  <si>
-    <t>lifeStage_count_a</t>
-  </si>
-  <si>
-    <t>lifeStage_count_e</t>
-  </si>
-  <si>
-    <t>lifeStage_count_l</t>
-  </si>
-  <si>
-    <t>decimalLatitude</t>
-  </si>
-  <si>
-    <t>decimalLongitude</t>
-  </si>
-  <si>
-    <t>verbatimCoordinates</t>
-  </si>
-  <si>
-    <t>verbatimLatitude</t>
-  </si>
-  <si>
-    <t>verbatimLongitude</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>eventID</t>
-  </si>
-  <si>
-    <t>individualCount</t>
-  </si>
-  <si>
-    <t>verbatimElevation</t>
-  </si>
-  <si>
-    <t>identificationVerificationStatus</t>
-  </si>
-  <si>
-    <t>entryDate</t>
-  </si>
-  <si>
-    <t>not DwC</t>
-  </si>
-  <si>
-    <t>behavior</t>
-  </si>
-  <si>
-    <t>Belgium2: is not the only info present (also vitality and comments)</t>
-  </si>
-  <si>
-    <t>samplingMethod</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>county</t>
-  </si>
-  <si>
-    <t>accessRights</t>
-  </si>
-  <si>
-    <t>embargoDate</t>
-  </si>
-  <si>
-    <t>occurrenceRemarks</t>
-  </si>
-  <si>
-    <t>coordinateUncertaintyInMeters</t>
-  </si>
-  <si>
-    <t>deliveryDate</t>
-  </si>
-  <si>
-    <t>samplingProtocol</t>
-  </si>
-  <si>
-    <t>eventType</t>
-  </si>
-  <si>
-    <t>gridRef</t>
-  </si>
-  <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>nameAccordingTo</t>
-  </si>
-  <si>
-    <t>namePublishedInYear</t>
-  </si>
-  <si>
-    <t>Jahr</t>
-  </si>
-  <si>
-    <t>associatedMedia</t>
-  </si>
-  <si>
-    <t>recordedByID</t>
-  </si>
-  <si>
-    <t>eventDateUncertainty</t>
-  </si>
-  <si>
-    <t>eventTime</t>
-  </si>
-  <si>
-    <t>samplingEffort</t>
-  </si>
-  <si>
-    <t>municipalityID</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>degreeOfEstablishment</t>
-  </si>
-  <si>
-    <t>datasetName</t>
-  </si>
-  <si>
-    <t>species_id</t>
-  </si>
-  <si>
-    <t>srt_scientific</t>
-  </si>
-  <si>
-    <t>cbs_species_id</t>
-  </si>
-  <si>
-    <t>Beleidsstatus</t>
-  </si>
-  <si>
-    <t>for STELI and OPIE taxon is longer, for Netherlands scientific name comes from other file (merged)</t>
-  </si>
-  <si>
-    <t>occurrenceID</t>
-  </si>
-  <si>
-    <t>Location_name</t>
-  </si>
-  <si>
-    <t>habitat_aqua_1</t>
-  </si>
-  <si>
-    <t>vegetation_aqua_1</t>
-  </si>
-  <si>
-    <t>rives_aqua_1</t>
-  </si>
-  <si>
-    <t>habitat_aqua_2</t>
-  </si>
-  <si>
-    <t>eau_aqua_2</t>
-  </si>
-  <si>
-    <t>vegetation_aqua_2</t>
-  </si>
-  <si>
-    <t>rives_aqua_2</t>
-  </si>
-  <si>
-    <t>habitat_aqua_3</t>
-  </si>
-  <si>
-    <t>eau_aqua_3</t>
-  </si>
-  <si>
-    <t>vegetation_aqua_3</t>
-  </si>
-  <si>
-    <t>rives_aqua_3</t>
-  </si>
-  <si>
-    <t>habitat_terre_1</t>
-  </si>
-  <si>
-    <t>habitat_terre_2</t>
-  </si>
-  <si>
-    <t>habitat_terre_3</t>
-  </si>
-  <si>
-    <t>activites_humaines</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1046,8 @@
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1064,7 +1061,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1091,36 +1088,36 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1129,33 +1126,33 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1168,10 +1165,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1184,12 +1181,12 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1200,7 +1197,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1208,28 +1205,27 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>35</v>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1237,25 +1233,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1266,40 +1262,40 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>213</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1308,30 +1304,30 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1339,23 +1335,23 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>215</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1363,23 +1359,23 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>214</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1387,7 +1383,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1395,22 +1391,22 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1421,12 +1417,12 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1434,26 +1430,26 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1461,38 +1457,38 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>223</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1501,18 +1497,18 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1521,18 +1517,18 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>45</v>
+        <v>224</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>74</v>
+        <v>224</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1541,7 +1537,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1551,18 +1547,18 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1570,34 +1566,34 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1605,17 +1601,17 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1624,19 +1620,19 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1644,17 +1640,17 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1662,76 +1658,76 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>86</v>
+        <v>217</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1739,14 +1735,14 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1757,19 +1753,19 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>92</v>
+        <v>218</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1777,19 +1773,19 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>97</v>
+        <v>219</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1797,15 +1793,15 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1815,7 +1811,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1823,7 +1819,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -1831,15 +1827,15 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1849,12 +1845,12 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1865,27 +1861,27 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1894,16 +1890,16 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1912,21 +1908,21 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1934,77 +1930,77 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>103</v>
+        <v>220</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>107</v>
+        <v>221</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2015,12 +2011,12 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2028,12 +2024,12 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2047,44 +2043,44 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="I52" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2093,99 +2089,99 @@
         <v>11</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>12</v>
+        <v>222</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="F57" s="1"/>
       <c r="J57" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2193,16 +2189,16 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2210,16 +2206,16 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2228,16 +2224,16 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2246,16 +2242,16 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2264,16 +2260,16 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2282,16 +2278,16 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2300,16 +2296,16 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2318,16 +2314,16 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2336,16 +2332,16 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2354,16 +2350,16 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2372,16 +2368,16 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2390,16 +2386,16 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2407,32 +2403,32 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="H73" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2440,16 +2436,16 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2457,110 +2453,110 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted coordinates to WKT
</commit_message>
<xml_diff>
--- a/outputs/column_names.xlsx
+++ b/outputs/column_names.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="226">
   <si>
     <t>Austria</t>
   </si>
@@ -333,394 +333,397 @@
     <t>Location</t>
   </si>
   <si>
+    <t>validateur_atlas</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>id_site</t>
+  </si>
+  <si>
+    <t>date_validation_atlas</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>Location.name</t>
+  </si>
+  <si>
+    <t>nom_site</t>
+  </si>
+  <si>
+    <t>submunicipality</t>
+  </si>
+  <si>
+    <t>Recorders</t>
+  </si>
+  <si>
+    <t>habitat aqua 1</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>eau aqua 1</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>vegetation aqua 1</t>
+  </si>
+  <si>
+    <t>certain</t>
+  </si>
+  <si>
+    <t>rives aqua 1</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>habitat aqua 2</t>
+  </si>
+  <si>
+    <t>embargo_date</t>
+  </si>
+  <si>
+    <t>eau aqua 2</t>
+  </si>
+  <si>
+    <t>permission_observer</t>
+  </si>
+  <si>
+    <t>vegetation aqua 2</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>rives aqua 2</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>habitat aqua 3</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>eau aqua 3</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
+  </si>
+  <si>
+    <t>vegetation aqua 3</t>
+  </si>
+  <si>
+    <t>id_species</t>
+  </si>
+  <si>
+    <t>rives aqua 3</t>
+  </si>
+  <si>
+    <t>id_species_type</t>
+  </si>
+  <si>
+    <t>habitat terre 1</t>
+  </si>
+  <si>
+    <t>id_checklist</t>
+  </si>
+  <si>
+    <t>habitat terre 2</t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>habitat terre 3</t>
+  </si>
+  <si>
+    <t>type_transect</t>
+  </si>
+  <si>
+    <t>activites humaines</t>
+  </si>
+  <si>
+    <t>vent</t>
+  </si>
+  <si>
+    <t>lon centroid site</t>
+  </si>
+  <si>
+    <t>lat centroid site</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>scientificName</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>vernacularName</t>
+  </si>
+  <si>
+    <t>recordedBy</t>
+  </si>
+  <si>
+    <t>scientificNameID</t>
+  </si>
+  <si>
+    <t>eventDate</t>
+  </si>
+  <si>
+    <t>lifeStage</t>
+  </si>
+  <si>
+    <t>lifeStage_count_a</t>
+  </si>
+  <si>
+    <t>lifeStage_count_e</t>
+  </si>
+  <si>
+    <t>lifeStage_count_l</t>
+  </si>
+  <si>
+    <t>decimalLatitude</t>
+  </si>
+  <si>
+    <t>decimalLongitude</t>
+  </si>
+  <si>
+    <t>verbatimCoordinates</t>
+  </si>
+  <si>
+    <t>verbatimLatitude</t>
+  </si>
+  <si>
+    <t>verbatimLongitude</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>eventID</t>
+  </si>
+  <si>
+    <t>individualCount</t>
+  </si>
+  <si>
+    <t>verbatimElevation</t>
+  </si>
+  <si>
+    <t>identificationVerificationStatus</t>
+  </si>
+  <si>
+    <t>entryDate</t>
+  </si>
+  <si>
+    <t>not DwC</t>
+  </si>
+  <si>
+    <t>behavior</t>
+  </si>
+  <si>
+    <t>Belgium2: is not the only info present (also vitality and comments)</t>
+  </si>
+  <si>
+    <t>samplingMethod</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>accessRights</t>
+  </si>
+  <si>
+    <t>embargoDate</t>
+  </si>
+  <si>
+    <t>occurrenceRemarks</t>
+  </si>
+  <si>
+    <t>coordinateUncertaintyInMeters</t>
+  </si>
+  <si>
+    <t>deliveryDate</t>
+  </si>
+  <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>gridRef</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>nameAccordingTo</t>
+  </si>
+  <si>
+    <t>namePublishedInYear</t>
+  </si>
+  <si>
+    <t>Jahr</t>
+  </si>
+  <si>
+    <t>associatedMedia</t>
+  </si>
+  <si>
+    <t>recordedByID</t>
+  </si>
+  <si>
+    <t>eventDateUncertainty</t>
+  </si>
+  <si>
+    <t>eventTime</t>
+  </si>
+  <si>
+    <t>samplingEffort</t>
+  </si>
+  <si>
+    <t>municipalityID</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>degreeOfEstablishment</t>
+  </si>
+  <si>
+    <t>datasetName</t>
+  </si>
+  <si>
+    <t>species_id</t>
+  </si>
+  <si>
+    <t>srt_scientific</t>
+  </si>
+  <si>
+    <t>cbs_species_id</t>
+  </si>
+  <si>
+    <t>Beleidsstatus</t>
+  </si>
+  <si>
+    <t>for STELI and OPIE taxon is longer, for Netherlands scientific name comes from other file (merged)</t>
+  </si>
+  <si>
+    <t>occurrenceID</t>
+  </si>
+  <si>
+    <t>Location_name</t>
+  </si>
+  <si>
+    <t>habitat_aqua_1</t>
+  </si>
+  <si>
+    <t>vegetation_aqua_1</t>
+  </si>
+  <si>
+    <t>rives_aqua_1</t>
+  </si>
+  <si>
+    <t>habitat_aqua_2</t>
+  </si>
+  <si>
+    <t>eau_aqua_2</t>
+  </si>
+  <si>
+    <t>vegetation_aqua_2</t>
+  </si>
+  <si>
+    <t>rives_aqua_2</t>
+  </si>
+  <si>
+    <t>habitat_aqua_3</t>
+  </si>
+  <si>
+    <t>eau_aqua_3</t>
+  </si>
+  <si>
+    <t>vegetation_aqua_3</t>
+  </si>
+  <si>
+    <t>rives_aqua_3</t>
+  </si>
+  <si>
+    <t>habitat_terre_1</t>
+  </si>
+  <si>
+    <t>habitat_terre_2</t>
+  </si>
+  <si>
+    <t>habitat_terre_3</t>
+  </si>
+  <si>
+    <t>activites_humaines</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>E dec deg</t>
+  </si>
+  <si>
+    <t>N dec deg</t>
+  </si>
+  <si>
+    <t>E deg min sec</t>
+  </si>
+  <si>
+    <t>N deg min sec</t>
+  </si>
+  <si>
+    <t>Location name</t>
+  </si>
+  <si>
+    <t>Altitude m asl</t>
+  </si>
+  <si>
+    <t>Ref no</t>
+  </si>
+  <si>
+    <t>Adult total</t>
+  </si>
+  <si>
+    <t>Exuviae</t>
+  </si>
+  <si>
+    <t>verbatimTaxonRank</t>
+  </si>
+  <si>
+    <t>geometry_site</t>
+  </si>
+  <si>
+    <t>coordonnees observation</t>
+  </si>
+  <si>
     <t>protocole</t>
   </si>
   <si>
-    <t>validateur_atlas</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>id_site</t>
-  </si>
-  <si>
-    <t>date_validation_atlas</t>
-  </si>
-  <si>
-    <t>municipality</t>
-  </si>
-  <si>
-    <t>Location.name</t>
-  </si>
-  <si>
-    <t>nom_site</t>
-  </si>
-  <si>
-    <t>submunicipality</t>
-  </si>
-  <si>
-    <t>Recorders</t>
-  </si>
-  <si>
-    <t>habitat aqua 1</t>
-  </si>
-  <si>
-    <t>province</t>
-  </si>
-  <si>
-    <t>eau aqua 1</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>vegetation aqua 1</t>
-  </si>
-  <si>
-    <t>certain</t>
-  </si>
-  <si>
-    <t>rives aqua 1</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>habitat aqua 2</t>
-  </si>
-  <si>
-    <t>embargo_date</t>
-  </si>
-  <si>
-    <t>eau aqua 2</t>
-  </si>
-  <si>
-    <t>permission_observer</t>
-  </si>
-  <si>
-    <t>vegetation aqua 2</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>rives aqua 2</t>
-  </si>
-  <si>
-    <t>precision</t>
-  </si>
-  <si>
-    <t>habitat aqua 3</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>eau aqua 3</t>
-  </si>
-  <si>
-    <t>delivery_date</t>
-  </si>
-  <si>
-    <t>vegetation aqua 3</t>
-  </si>
-  <si>
-    <t>id_species</t>
-  </si>
-  <si>
-    <t>rives aqua 3</t>
-  </si>
-  <si>
-    <t>id_species_type</t>
-  </si>
-  <si>
-    <t>habitat terre 1</t>
-  </si>
-  <si>
-    <t>id_checklist</t>
-  </si>
-  <si>
-    <t>habitat terre 2</t>
-  </si>
-  <si>
-    <t>transect</t>
-  </si>
-  <si>
-    <t>habitat terre 3</t>
-  </si>
-  <si>
-    <t>type_transect</t>
-  </si>
-  <si>
-    <t>activites humaines</t>
-  </si>
-  <si>
-    <t>vent</t>
-  </si>
-  <si>
-    <t>lon centroid site</t>
-  </si>
-  <si>
-    <t>lat centroid site</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>scientificName</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>taxonRank</t>
-  </si>
-  <si>
-    <t>Use controlled vocabulary (cf DwC page); usually will be species</t>
-  </si>
-  <si>
-    <t>vernacularName</t>
-  </si>
-  <si>
-    <t>recordedBy</t>
-  </si>
-  <si>
-    <t>scientificNameID</t>
-  </si>
-  <si>
-    <t>eventDate</t>
-  </si>
-  <si>
-    <t>lifeStage</t>
-  </si>
-  <si>
-    <t>lifeStage_count_a</t>
-  </si>
-  <si>
-    <t>lifeStage_count_e</t>
-  </si>
-  <si>
-    <t>lifeStage_count_l</t>
-  </si>
-  <si>
-    <t>decimalLatitude</t>
-  </si>
-  <si>
-    <t>decimalLongitude</t>
-  </si>
-  <si>
-    <t>verbatimCoordinates</t>
-  </si>
-  <si>
-    <t>verbatimLatitude</t>
-  </si>
-  <si>
-    <t>verbatimLongitude</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>eventID</t>
-  </si>
-  <si>
-    <t>individualCount</t>
-  </si>
-  <si>
-    <t>verbatimElevation</t>
-  </si>
-  <si>
-    <t>identificationVerificationStatus</t>
-  </si>
-  <si>
-    <t>entryDate</t>
-  </si>
-  <si>
-    <t>not DwC</t>
-  </si>
-  <si>
-    <t>behavior</t>
-  </si>
-  <si>
-    <t>Belgium2: is not the only info present (also vitality and comments)</t>
-  </si>
-  <si>
-    <t>samplingMethod</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>county</t>
-  </si>
-  <si>
-    <t>accessRights</t>
-  </si>
-  <si>
-    <t>embargoDate</t>
-  </si>
-  <si>
-    <t>occurrenceRemarks</t>
-  </si>
-  <si>
-    <t>coordinateUncertaintyInMeters</t>
-  </si>
-  <si>
-    <t>deliveryDate</t>
-  </si>
-  <si>
-    <t>samplingProtocol</t>
-  </si>
-  <si>
-    <t>eventType</t>
-  </si>
-  <si>
-    <t>gridRef</t>
-  </si>
-  <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>nameAccordingTo</t>
-  </si>
-  <si>
-    <t>namePublishedInYear</t>
-  </si>
-  <si>
-    <t>Jahr</t>
-  </si>
-  <si>
-    <t>associatedMedia</t>
-  </si>
-  <si>
-    <t>recordedByID</t>
-  </si>
-  <si>
-    <t>eventDateUncertainty</t>
-  </si>
-  <si>
-    <t>eventTime</t>
-  </si>
-  <si>
-    <t>samplingEffort</t>
-  </si>
-  <si>
-    <t>municipalityID</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>degreeOfEstablishment</t>
-  </si>
-  <si>
-    <t>datasetName</t>
-  </si>
-  <si>
-    <t>species_id</t>
-  </si>
-  <si>
-    <t>srt_scientific</t>
-  </si>
-  <si>
-    <t>cbs_species_id</t>
-  </si>
-  <si>
-    <t>Beleidsstatus</t>
-  </si>
-  <si>
-    <t>for STELI and OPIE taxon is longer, for Netherlands scientific name comes from other file (merged)</t>
-  </si>
-  <si>
-    <t>occurrenceID</t>
-  </si>
-  <si>
-    <t>Location_name</t>
-  </si>
-  <si>
-    <t>habitat_aqua_1</t>
-  </si>
-  <si>
-    <t>vegetation_aqua_1</t>
-  </si>
-  <si>
-    <t>rives_aqua_1</t>
-  </si>
-  <si>
-    <t>habitat_aqua_2</t>
-  </si>
-  <si>
-    <t>eau_aqua_2</t>
-  </si>
-  <si>
-    <t>vegetation_aqua_2</t>
-  </si>
-  <si>
-    <t>rives_aqua_2</t>
-  </si>
-  <si>
-    <t>habitat_aqua_3</t>
-  </si>
-  <si>
-    <t>eau_aqua_3</t>
-  </si>
-  <si>
-    <t>vegetation_aqua_3</t>
-  </si>
-  <si>
-    <t>rives_aqua_3</t>
-  </si>
-  <si>
-    <t>habitat_terre_1</t>
-  </si>
-  <si>
-    <t>habitat_terre_2</t>
-  </si>
-  <si>
-    <t>habitat_terre_3</t>
-  </si>
-  <si>
-    <t>activites_humaines</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>E dec deg</t>
-  </si>
-  <si>
-    <t>N dec deg</t>
-  </si>
-  <si>
-    <t>E deg min sec</t>
-  </si>
-  <si>
-    <t>N deg min sec</t>
-  </si>
-  <si>
-    <t>Location name</t>
-  </si>
-  <si>
-    <t>Altitude m asl</t>
-  </si>
-  <si>
-    <t>Ref no</t>
-  </si>
-  <si>
-    <t>Adult total</t>
-  </si>
-  <si>
-    <t>Exuviae</t>
+    <t>decimalCoordinates</t>
   </si>
 </sst>
 </file>
@@ -1043,11 +1046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1061,7 +1064,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1088,12 +1091,12 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
@@ -1107,7 +1110,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
@@ -1117,7 +1120,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1135,7 +1138,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>26</v>
@@ -1144,15 +1147,15 @@
         <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1165,10 +1168,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1181,12 +1184,12 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1197,7 +1200,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>221</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1208,13 +1211,11 @@
       <c r="H7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>144</v>
-      </c>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -1233,12 +1234,12 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1251,7 +1252,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1271,7 +1272,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -1282,7 +1283,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
@@ -1295,7 +1296,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1348,7 +1349,7 @@
         <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>32</v>
@@ -1372,7 +1373,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>36</v>
@@ -1383,7 +1384,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1396,7 +1397,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1417,7 +1418,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1430,12 +1431,12 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1457,7 +1458,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1477,7 +1478,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>35</v>
@@ -1488,7 +1489,7 @@
         <v>30</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1497,7 +1498,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>41</v>
@@ -1517,7 +1518,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
@@ -1525,10 +1526,10 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1537,7 +1538,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1553,7 +1554,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1566,12 +1567,12 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>52</v>
@@ -1579,7 +1580,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1593,7 +1594,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1611,7 +1612,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1627,7 +1628,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1640,17 +1641,17 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1658,12 +1659,12 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>76</v>
@@ -1676,12 +1677,9 @@
         <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="I31" s="1" t="s">
         <v>45</v>
       </c>
@@ -1689,7 +1687,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>81</v>
@@ -1702,12 +1700,9 @@
         <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="I32" s="1" t="s">
         <v>40</v>
       </c>
@@ -1715,77 +1710,74 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1793,66 +1785,70 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -1861,45 +1857,43 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>187</v>
+        <v>100</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1" t="s">
-        <v>164</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1908,165 +1902,167 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>104</v>
+        <v>184</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>220</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="J45" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F46" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
+      <c r="I48" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>77</v>
@@ -2080,7 +2076,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2089,63 +2085,63 @@
         <v>11</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F57" s="1"/>
       <c r="J57" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -2160,28 +2156,28 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2189,16 +2185,16 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2206,11 +2202,11 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -2228,7 +2224,7 @@
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -2246,12 +2242,12 @@
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2260,11 +2256,11 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
@@ -2282,12 +2278,12 @@
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2296,16 +2292,16 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2314,16 +2310,16 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2332,16 +2328,16 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2350,16 +2346,16 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2368,16 +2364,16 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2386,16 +2382,16 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2403,32 +2399,32 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="H73" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2436,16 +2432,16 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2453,110 +2449,142 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>164</v>
+        <v>224</v>
+      </c>
+      <c r="H83" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>164</v>
+        <v>222</v>
+      </c>
+      <c r="H84" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>